<commit_message>
Añadida paginacion al reporte PDF
</commit_message>
<xml_diff>
--- a/activosFijos.xlsx
+++ b/activosFijos.xlsx
@@ -47,28 +47,28 @@
     <t>Activo 1</t>
   </si>
   <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>Descripción 1</t>
-  </si>
-  <si>
-    <t>Tipo 1</t>
-  </si>
-  <si>
-    <t>Marca 1</t>
-  </si>
-  <si>
-    <t>Activo 2</t>
-  </si>
-  <si>
-    <t>Descripción 2</t>
-  </si>
-  <si>
-    <t>Tipo 2</t>
-  </si>
-  <si>
-    <t>Marca 2</t>
+    <t>15-01-2023</t>
+  </si>
+  <si>
+    <t>Descripción del Activo 1</t>
+  </si>
+  <si>
+    <t>Equipo de Oficina</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Monitor 2k</t>
+  </si>
+  <si>
+    <t>18-10-2023</t>
+  </si>
+  <si>
+    <t>Monitor de alta resolucion</t>
+  </si>
+  <si>
+    <t>Puma</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>100.0</v>
+        <v>1000.0</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -177,42 +177,42 @@
         <v>10.0</v>
       </c>
       <c r="I2" t="n">
-        <v>10.0</v>
+        <v>66.67</v>
       </c>
       <c r="J2" t="n">
-        <v>90.0</v>
+        <v>933.33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>200.0</v>
+        <v>1500.0</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
       </c>
       <c r="H3" t="n">
-        <v>15.0</v>
+        <v>10.0</v>
       </c>
       <c r="I3" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="J3" t="n">
-        <v>170.0</v>
+        <v>1500.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando sql de inserts
</commit_message>
<xml_diff>
--- a/activosFijos.xlsx
+++ b/activosFijos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -59,46 +59,37 @@
     <t>Valor actual</t>
   </si>
   <si>
-    <t>Activo 1</t>
-  </si>
-  <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>Descripción 1</t>
-  </si>
-  <si>
-    <t>Tipo 1</t>
-  </si>
-  <si>
-    <t>Marca 1</t>
-  </si>
-  <si>
-    <t>Calle 1</t>
-  </si>
-  <si>
-    <t>Avenida 1</t>
-  </si>
-  <si>
-    <t>Bloque 1</t>
-  </si>
-  <si>
-    <t>La Paz</t>
-  </si>
-  <si>
-    <t>Personal 1</t>
-  </si>
-  <si>
-    <t>Activo 2</t>
-  </si>
-  <si>
-    <t>Descripción 2</t>
-  </si>
-  <si>
-    <t>Tipo 2</t>
-  </si>
-  <si>
-    <t>Marca 2</t>
+    <t>Meses restantes</t>
+  </si>
+  <si>
+    <t>Mesa de Trabajo</t>
+  </si>
+  <si>
+    <t>10-03-2023</t>
+  </si>
+  <si>
+    <t>Mesa de oficina</t>
+  </si>
+  <si>
+    <t>Animales de trabajo</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>Calle Rosales</t>
+  </si>
+  <si>
+    <t>Avenida Ávila Camacho</t>
+  </si>
+  <si>
+    <t>Area Amarilla</t>
+  </si>
+  <si>
+    <t>El Alto</t>
+  </si>
+  <si>
+    <t>Luisa Martínez</t>
   </si>
 </sst>
 </file>
@@ -143,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,99 +186,58 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>100.0</v>
+        <v>400.25</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="n">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="N2" t="n">
-        <v>10.0</v>
+        <v>75.05</v>
       </c>
       <c r="O2" t="n">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>170.0</v>
+        <v>325.2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>39.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>